<commit_message>
cube implementation - draft 1
</commit_message>
<xml_diff>
--- a/doc/EnterpriseBusMatrix.xlsx
+++ b/doc/EnterpriseBusMatrix.xlsx
@@ -83,10 +83,10 @@
     <t>Scene Location</t>
   </si>
   <si>
-    <t>Disposition Location</t>
-  </si>
-  <si>
     <t>Maintenance Event</t>
+  </si>
+  <si>
+    <t>Transport Location</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <dimension ref="A2:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +484,7 @@
         <v>18</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>9</v>
@@ -505,7 +505,7 @@
         <v>15</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>